<commit_message>
Added AS5048A check program and RMP Formula New check program for AS5048A checks the distance between AS5048A and the magnet. RPM formula converts the RPM to the Microstepping period.
</commit_message>
<xml_diff>
--- a/Formulas.xlsx
+++ b/Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459D2362-5F9E-4053-AB27-36D390655C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5DD1EF-32B3-43E0-9856-9884303CDAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Motor_RPM</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Microsteps_per_Second</t>
+  </si>
+  <si>
+    <t>Microsteps_Period</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   <dimension ref="B2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -517,7 +520,7 @@
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>0.13700000000000001</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -578,11 +581,11 @@
     <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6">
         <f>B3/C3</f>
-        <v>6.8500000000000002E-3</v>
+        <v>0.05</v>
       </c>
       <c r="C6">
         <f>B3/C3 * 60 *24</f>
-        <v>9.8640000000000008</v>
+        <v>72</v>
       </c>
       <c r="D6">
         <f>D3*E3</f>
@@ -590,7 +593,7 @@
       </c>
       <c r="E6">
         <f>(B3/C3)*60*24*D3*E3</f>
-        <v>2.4858870967741939</v>
+        <v>18.145161290322584</v>
       </c>
       <c r="G6">
         <f>I3/H3</f>
@@ -611,6 +614,29 @@
       <c r="K6" s="2">
         <f>(J6*K3)/60</f>
         <v>117.57037037037038</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>51200</v>
+      </c>
+      <c r="D9">
+        <f>(B9*C9)/(60*0.715)</f>
+        <v>1193.4731934731935</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Changed Perfusion library and minor bug fixes
</commit_message>
<xml_diff>
--- a/Formulas.xlsx
+++ b/Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5DD1EF-32B3-43E0-9856-9884303CDAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A77E504-92FB-4666-A34D-341A944202BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Motor_RPM</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Microsteps_Period</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>Verification_Microsteps_Period</t>
   </si>
 </sst>
 </file>
@@ -472,7 +478,7 @@
   <dimension ref="B2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -520,7 +526,7 @@
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>1</v>
+        <v>0.13780000000000001</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -581,11 +587,11 @@
     <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6">
         <f>B3/C3</f>
-        <v>0.05</v>
+        <v>6.8900000000000003E-3</v>
       </c>
       <c r="C6">
         <f>B3/C3 * 60 *24</f>
-        <v>72</v>
+        <v>9.9215999999999998</v>
       </c>
       <c r="D6">
         <f>D3*E3</f>
@@ -593,7 +599,7 @@
       </c>
       <c r="E6">
         <f>(B3/C3)*60*24*D3*E3</f>
-        <v>18.145161290322584</v>
+        <v>2.5004032258064517</v>
       </c>
       <c r="G6">
         <f>I3/H3</f>
@@ -637,6 +643,35 @@
       <c r="D9">
         <f>(B9*C9)/(60*0.715)</f>
         <v>1193.4731934731935</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="H10">
+        <f>(G3*H3*J3*K3/(1440*60*0.715*I3))</f>
+        <v>164.43408443408444</v>
+      </c>
+      <c r="I10">
+        <f>(H3*J3*K3/(1440*60*0.715*I3))</f>
+        <v>65.773633773633776</v>
+      </c>
+      <c r="J10">
+        <f>I10*G10</f>
+        <v>6.5773633773633779</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.35">
@@ -673,6 +708,10 @@
       <c r="D14">
         <f>K6</f>
         <v>117.57037037037038</v>
+      </c>
+      <c r="G14">
+        <f>4.96/(1.25*20)</f>
+        <v>0.19839999999999999</v>
       </c>
     </row>
     <row r="22" spans="5:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Calculations changed for TMC controller
</commit_message>
<xml_diff>
--- a/Formulas.xlsx
+++ b/Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F44F14-4AB7-4575-814F-BE1B1BC80F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FC5444-5380-487C-B9DF-C2DF3D6537B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="B2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,7 +582,7 @@
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>0.13780000000000001</v>
+        <v>0.1694</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -591,14 +591,14 @@
         <v>1.25</v>
       </c>
       <c r="E3">
-        <f>1/4.96</f>
-        <v>0.20161290322580647</v>
+        <f>0.205/D3</f>
+        <v>0.16399999999999998</v>
       </c>
       <c r="G3">
         <v>2.5</v>
       </c>
       <c r="H3">
-        <v>4.96</v>
+        <v>6.1</v>
       </c>
       <c r="I3">
         <v>1.25</v>
@@ -643,39 +643,39 @@
     <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6">
         <f>B3/C3</f>
-        <v>6.8900000000000003E-3</v>
+        <v>8.4700000000000001E-3</v>
       </c>
       <c r="C6">
         <f>B3/C3 * 60 *24</f>
-        <v>9.9215999999999998</v>
+        <v>12.1968</v>
       </c>
       <c r="D6">
         <f>D3*E3</f>
-        <v>0.25201612903225806</v>
+        <v>0.20499999999999996</v>
       </c>
       <c r="E6">
         <f>(B3/C3)*60*24*D3*E3</f>
-        <v>2.5004032258064517</v>
+        <v>2.5003439999999997</v>
       </c>
       <c r="G6">
         <f>I3/H3</f>
-        <v>0.25201612903225806</v>
+        <v>0.20491803278688525</v>
       </c>
       <c r="H6">
         <f>G3/(I3/H3)</f>
-        <v>9.92</v>
+        <v>12.2</v>
       </c>
       <c r="I6">
         <f>H6/1440</f>
-        <v>6.8888888888888888E-3</v>
+        <v>8.4722222222222213E-3</v>
       </c>
       <c r="J6">
         <f>I6*J3</f>
-        <v>0.13777777777777778</v>
+        <v>0.16944444444444443</v>
       </c>
       <c r="K6" s="2">
         <f>(J6*K3)/60</f>
-        <v>117.57037037037038</v>
+        <v>144.59259259259258</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
@@ -719,15 +719,15 @@
       </c>
       <c r="H10">
         <f>(G3*H3*J3*K3/(1440*60*0.715*I3))</f>
-        <v>164.43408443408444</v>
+        <v>202.22740222740222</v>
       </c>
       <c r="I10">
         <f>(H3*J3*K3/(1440*60*0.715*I3))</f>
-        <v>65.773633773633776</v>
+        <v>80.890960890960898</v>
       </c>
       <c r="J10">
         <f>I10*G10</f>
-        <v>6.5773633773633779</v>
+        <v>8.0890960890960901</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.35">
@@ -756,14 +756,14 @@
     <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="2">
         <f>D14/C14</f>
-        <v>164.43408443408447</v>
+        <v>202.22740222740222</v>
       </c>
       <c r="C14">
         <v>0.71499999999999997</v>
       </c>
       <c r="D14">
         <f>K6</f>
-        <v>117.57037037037038</v>
+        <v>144.59259259259258</v>
       </c>
       <c r="G14">
         <f>4.96/(1.25*20)</f>

</xml_diff>

<commit_message>
More Measurements and formulas added.
</commit_message>
<xml_diff>
--- a/Formulas.xlsx
+++ b/Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FC5444-5380-487C-B9DF-C2DF3D6537B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730DB24B-6CE7-4A75-811C-4C88E29FC1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Motor_RPM</t>
   </si>
@@ -109,6 +109,39 @@
   </si>
   <si>
     <t>Volume 24h (mL)</t>
+  </si>
+  <si>
+    <t>1 Rotation distance (mm)</t>
+  </si>
+  <si>
+    <t>Inner-Radius (mm)</t>
+  </si>
+  <si>
+    <t>Rotations per mL</t>
+  </si>
+  <si>
+    <t>Volume per Day (mL)</t>
+  </si>
+  <si>
+    <t>Rotations requered per day</t>
+  </si>
+  <si>
+    <t>Volume per Rotation (mL/rot)</t>
+  </si>
+  <si>
+    <t>mm per mL</t>
+  </si>
+  <si>
+    <t>Rotations per Day</t>
+  </si>
+  <si>
+    <t>motor rpm</t>
+  </si>
+  <si>
+    <t>steps per sec</t>
+  </si>
+  <si>
+    <t>microsteps period</t>
   </si>
 </sst>
 </file>
@@ -159,15 +192,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -236,7 +279,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{738C273D-3CF8-4253-B808-4A3E1E13412E}" name="Table5" displayName="Table5" ref="G9:J10" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{738C273D-3CF8-4253-B808-4A3E1E13412E}" name="Table5" displayName="Table5" ref="G9:J11" totalsRowCount="1">
   <autoFilter ref="G9:J10" xr:uid="{738C273D-3CF8-4253-B808-4A3E1E13412E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{712D2897-2D76-4BC9-B598-55180B1E6D7D}" name="Desired_Flow (mL_per_Day)"/>
@@ -265,6 +308,54 @@
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7387B3BE-58E7-4EA7-AFA2-5D40D41F47DC}" name="Table7" displayName="Table7" ref="B24:G25" totalsRowShown="0">
+  <autoFilter ref="B24:G25" xr:uid="{7387B3BE-58E7-4EA7-AFA2-5D40D41F47DC}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{F9C8E740-AD58-4C81-B470-DB308309C8CA}" name="1 Rotation distance (mm)"/>
+    <tableColumn id="2" xr3:uid="{D43C6EEA-5A04-40B2-A4F7-F4DACF10486E}" name="Inner-Radius (mm)"/>
+    <tableColumn id="3" xr3:uid="{FC643971-5597-4662-9C63-6F60D0E2C3FF}" name="mm per mL">
+      <calculatedColumnFormula>1000/(3.14159*(POWER(C25,2)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{57EBB1A5-463C-4AC2-B3D5-56767D31549E}" name="Rotations per mL">
+      <calculatedColumnFormula>D25/B25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{3BBE06F6-454D-482C-A49E-CE70427AAF44}" name="Volume per Day (mL)"/>
+    <tableColumn id="6" xr3:uid="{F812E8BA-C3BB-49BE-9CEA-F4D85AF8551F}" name="Rotations requered per day">
+      <calculatedColumnFormula>E25*F25</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B7D367A4-7E54-469D-A9E4-F44764D82BEF}" name="Table8" displayName="Table8" ref="D27:I28" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="D27:I28" xr:uid="{B7D367A4-7E54-469D-A9E4-F44764D82BEF}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A6C0BB03-5867-4013-885C-1D5FCF83F555}" name="Volume per Rotation (mL/rot)">
+      <calculatedColumnFormula>B25/D25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{8E186B87-3370-4994-9B85-7382A69DAC75}" name="Rotations per Day">
+      <calculatedColumnFormula>F25/D28</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{CCD0E4F0-F77A-416B-9CDB-59206E7D6697}" name="motor rpm">
+      <calculatedColumnFormula>E28/1440*20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{AD866146-2488-4CF5-B748-24CD3C88547C}" name="steps per sec">
+      <calculatedColumnFormula>(F28*K3)/60</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{62718193-0B05-49C1-90C1-FBF13473BA55}" name="microsteps period">
+      <calculatedColumnFormula>G28/C14</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{E2EE6A37-4F3D-4758-A497-4E6331BAE570}" name="Constant">
+      <calculatedColumnFormula>H28/F25</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -531,19 +622,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K27"/>
+  <dimension ref="B2:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="22.90625" customWidth="1"/>
     <col min="3" max="3" width="22.453125" customWidth="1"/>
-    <col min="4" max="4" width="23.81640625" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" customWidth="1"/>
     <col min="5" max="5" width="20.6328125" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
     <col min="7" max="7" width="26.26953125" customWidth="1"/>
     <col min="8" max="8" width="22.1796875" customWidth="1"/>
     <col min="9" max="9" width="27.08984375" customWidth="1"/>
@@ -781,7 +872,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="G17">
         <v>0.18</v>
       </c>
@@ -793,45 +884,121 @@
         <v>2.5411764705882351</v>
       </c>
     </row>
-    <row r="22" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="5:9" x14ac:dyDescent="0.35">
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="5:9" x14ac:dyDescent="0.35">
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>1.25</v>
+      </c>
+      <c r="C25">
+        <v>7.95</v>
+      </c>
+      <c r="D25">
+        <f>1000/(3.14159*(POWER(C25,2)))</f>
+        <v>5.0363538633578822</v>
+      </c>
+      <c r="E25" s="1">
+        <f>D25/B25</f>
+        <v>4.0290830906863055</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G25" s="1">
+        <f>E25*F25</f>
+        <v>10.072707726715764</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="5:9" x14ac:dyDescent="0.35">
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D28">
+        <f>B25/D25</f>
+        <v>0.24819542746874998</v>
+      </c>
+      <c r="E28">
+        <f>F25/D28</f>
+        <v>10.072707726715764</v>
+      </c>
+      <c r="F28">
+        <f>E28/1440*20</f>
+        <v>0.13989871842660784</v>
+      </c>
+      <c r="G28">
+        <f>(F28*K3)/60</f>
+        <v>119.38023972403867</v>
+      </c>
+      <c r="H28">
+        <f>G28/C14</f>
+        <v>166.96537024341075</v>
+      </c>
+      <c r="I28">
+        <f>H28/F25</f>
+        <v>66.786148097364304</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="6">
+  <tableParts count="8">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New reverse button functionality in the dashboard Reverse button added to the dashboard for adjusting syringe position. New Measurements added.
</commit_message>
<xml_diff>
--- a/Formulas.xlsx
+++ b/Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730DB24B-6CE7-4A75-811C-4C88E29FC1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDED9554-40E0-472D-9D07-A629CA845339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,6 +148,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,16 +195,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -209,6 +213,9 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -324,7 +331,7 @@
       <calculatedColumnFormula>D25/B25</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{3BBE06F6-454D-482C-A49E-CE70427AAF44}" name="Volume per Day (mL)"/>
-    <tableColumn id="6" xr3:uid="{F812E8BA-C3BB-49BE-9CEA-F4D85AF8551F}" name="Rotations requered per day">
+    <tableColumn id="6" xr3:uid="{F812E8BA-C3BB-49BE-9CEA-F4D85AF8551F}" name="Rotations requered per day" dataDxfId="1">
       <calculatedColumnFormula>E25*F25</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -625,7 +632,7 @@
   <dimension ref="B2:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -932,7 +939,7 @@
       <c r="F25" s="1">
         <v>2.5</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="4">
         <f>E25*F25</f>
         <v>10.072707726715764</v>
       </c>

</xml_diff>

<commit_message>
New Measurements added and formula improved
</commit_message>
<xml_diff>
--- a/Formulas.xlsx
+++ b/Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDED9554-40E0-472D-9D07-A629CA845339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E251377-A194-4822-8564-2F49C972452C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,7 +311,7 @@
     <tableColumn id="1" xr3:uid="{1901AE87-C543-460F-9299-F61BBCA4294C}" name="Motor_RPM"/>
     <tableColumn id="2" xr3:uid="{B12B22C6-DB86-4BC6-9744-CE33599A6746}" name="Motor_Steps_per_Revo"/>
     <tableColumn id="3" xr3:uid="{C92159EF-32B7-423E-9A09-14F8802E84F8}" name="Microsteps_Period">
-      <calculatedColumnFormula>(B9*C9)/(60*0.715)</calculatedColumnFormula>
+      <calculatedColumnFormula>(B9*C9)/(60*0.71525)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -632,7 +632,7 @@
   <dimension ref="B2:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -680,7 +680,7 @@
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>0.1694</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -689,14 +689,13 @@
         <v>1.25</v>
       </c>
       <c r="E3">
-        <f>0.205/D3</f>
-        <v>0.16399999999999998</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="G3">
         <v>2.5</v>
       </c>
       <c r="H3">
-        <v>6.1</v>
+        <v>5.04</v>
       </c>
       <c r="I3">
         <v>1.25</v>
@@ -741,39 +740,39 @@
     <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6">
         <f>B3/C3</f>
-        <v>8.4700000000000001E-3</v>
+        <v>7.000000000000001E-3</v>
       </c>
       <c r="C6">
         <f>B3/C3 * 60 *24</f>
-        <v>12.1968</v>
+        <v>10.080000000000002</v>
       </c>
       <c r="D6">
         <f>D3*E3</f>
-        <v>0.20499999999999996</v>
+        <v>0.2475</v>
       </c>
       <c r="E6">
         <f>(B3/C3)*60*24*D3*E3</f>
-        <v>2.5003439999999997</v>
+        <v>2.4948000000000006</v>
       </c>
       <c r="G6">
         <f>I3/H3</f>
-        <v>0.20491803278688525</v>
+        <v>0.24801587301587302</v>
       </c>
       <c r="H6">
         <f>G3/(I3/H3)</f>
-        <v>12.2</v>
+        <v>10.08</v>
       </c>
       <c r="I6">
         <f>H6/1440</f>
-        <v>8.4722222222222213E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="J6">
         <f>I6*J3</f>
-        <v>0.16944444444444443</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K6" s="2">
         <f>(J6*K3)/60</f>
-        <v>144.59259259259258</v>
+        <v>119.46666666666668</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
@@ -789,14 +788,14 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C9">
         <v>51200</v>
       </c>
       <c r="D9">
-        <f>(B9*C9)/(60*0.715)</f>
-        <v>1193.4731934731935</v>
+        <f>(B9*C9)/(60*0.71525)</f>
+        <v>167.02784574158218</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -813,19 +812,19 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="G10">
-        <v>0.1</v>
+        <v>2.5</v>
       </c>
       <c r="H10">
         <f>(G3*H3*J3*K3/(1440*60*0.715*I3))</f>
-        <v>202.22740222740222</v>
+        <v>167.08624708624708</v>
       </c>
       <c r="I10">
         <f>(H3*J3*K3/(1440*60*0.715*I3))</f>
-        <v>80.890960890960898</v>
+        <v>66.834498834498831</v>
       </c>
       <c r="J10">
         <f>I10*G10</f>
-        <v>8.0890960890960901</v>
+        <v>167.08624708624708</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.35">
@@ -854,14 +853,14 @@
     <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="2">
         <f>D14/C14</f>
-        <v>202.22740222740222</v>
+        <v>167.08624708624711</v>
       </c>
       <c r="C14">
         <v>0.71499999999999997</v>
       </c>
       <c r="D14">
         <f>K6</f>
-        <v>144.59259259259258</v>
+        <v>119.46666666666668</v>
       </c>
       <c r="G14">
         <f>4.96/(1.25*20)</f>

</xml_diff>